<commit_message>
Have train_and_save write model results to a csv.
</commit_message>
<xml_diff>
--- a/2016-05-11_data/models.xlsx
+++ b/2016-05-11_data/models.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
-    <sheet name="train" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
   <si>
     <t>kernel</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -59,18 +58,6 @@
   </si>
   <si>
     <t>hypers</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>structure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>log_mKate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hypers(var_n=0.31273769260395001, var_p=0.78982392252858546)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -671,7 +658,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -716,10 +703,10 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1">
         <v>-180.02799899999999</v>
@@ -734,18 +721,18 @@
         <v>0.52029999999999998</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1">
         <v>-181.224637</v>
@@ -760,15 +747,15 @@
         <v>0.51019999999999999</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1">
         <v>-180.85019800000001</v>
@@ -783,15 +770,15 @@
         <v>0.51270000000000004</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1">
         <v>-198.41727299999999</v>
@@ -806,15 +793,15 @@
         <v>0.51870000000000005</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1">
         <v>-229.12684200000001</v>
@@ -829,15 +816,15 @@
         <v>0.30730000000000002</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1">
         <v>-208.253334</v>
@@ -852,18 +839,18 @@
         <v>0.4889</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1">
         <v>-208.28059200000001</v>
@@ -878,15 +865,15 @@
         <v>0.48959999999999998</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1">
         <v>-208.46642399999999</v>
@@ -901,15 +888,15 @@
         <v>0.4884</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1">
         <v>-117.009406</v>
@@ -918,15 +905,15 @@
         <v>1</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1">
         <v>85.406706999999997</v>
@@ -935,15 +922,15 @@
         <v>0.73880000000000001</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1">
         <v>-84.250449000000003</v>
@@ -952,15 +939,15 @@
         <v>0.82640000000000002</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1">
         <v>-84.265415000000004</v>
@@ -969,18 +956,18 @@
         <v>0.81730000000000003</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1">
         <v>-81.371268999999998</v>
@@ -989,18 +976,18 @@
         <v>0.97350000000000003</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C15" s="1">
         <v>-91.414389999999997</v>
@@ -1009,18 +996,18 @@
         <v>0.99880000000000002</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C16" s="1">
         <v>-102.782557</v>
@@ -1029,18 +1016,18 @@
         <v>0.99870000000000003</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C17" s="1">
         <v>-117.009406</v>
@@ -1049,10 +1036,10 @@
         <v>1</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1069,75 +1056,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2">
-        <v>-148.93375</v>
-      </c>
-      <c r="D2">
-        <v>-138.40078</v>
-      </c>
-      <c r="E2">
-        <v>0.78210000000000002</v>
-      </c>
-      <c r="F2">
-        <v>0.57379999999999998</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>